<commit_message>
Update primary print templates
</commit_message>
<xml_diff>
--- a/data/print_templates/A__picking__single_carton.xlsx
+++ b/data/print_templates/A__picking__single_carton.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EdouardGonnu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EdouardGonnu/asf-wms/data/print_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00037732-DA5A-5245-B695-2FD777236815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74308F53-011D-1B46-96A0-C3389EEA5175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D41FDF60-E254-7C4C-BFC3-DDF9FE3B5742}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$28</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,6 +36,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -107,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,93 +139,47 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,59 +197,68 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2125739</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C56201C-C9CD-D6D3-36C2-6815F7A3DA09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="419100" y="101600"/>
-          <a:ext cx="1706639" cy="1422400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,174 +578,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF51C3FB-7A83-BF41-B717-28B03D752EA9}">
-  <dimension ref="A10:E29"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="1" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="6"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="11" scale="69" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update print templates with classic logo images
</commit_message>
<xml_diff>
--- a/data/print_templates/A__picking__single_carton.xlsx
+++ b/data/print_templates/A__picking__single_carton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EdouardGonnu/asf-wms/data/print_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74308F53-011D-1B46-96A0-C3389EEA5175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424FB8A6-A563-E64F-9043-825CC18F6D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D41FDF60-E254-7C4C-BFC3-DDF9FE3B5742}"/>
   </bookViews>
@@ -36,28 +36,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
-  <metadataTypes count="1">
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </valueMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -159,9 +137,6 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -180,6 +155,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,68 +175,59 @@
 </styleSheet>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
-</file>
-
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>0</v>
-    <v>5</v>
-  </rv>
-</rvData>
-</file>
-
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
-  </s>
-</rvStructures>
-</file>
-
-<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
-<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rel r:id="rId1"/>
-</richValueRels>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>72391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D14FDF0-8F88-FF60-9352-78274C566961}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="76200"/>
+          <a:ext cx="3949700" cy="1215391"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,7 +553,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,48 +563,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -652,10 +619,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -675,116 +642,116 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="7"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="7"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="7"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="8"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="7"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="7"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -792,5 +759,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" scale="69" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>